<commit_message>
Added in some country names/population data
</commit_message>
<xml_diff>
--- a/startup_analysis.xlsx
+++ b/startup_analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Avg_founding_funding" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Avg_founding_funding!$A$1:$B$214</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Avg_funding_cat!$A$1:$B$47</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Avg_funding_country!$A$1:$B$151</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Avg_funding_country!$A$1:$D$151</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Companies_per_category!$A$1:$B$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Country_count!$A$1:$B$151</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Num_founded_per_year!$A$1:$B$214</definedName>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="263">
   <si>
     <t>Year</t>
   </si>
@@ -641,14 +641,196 @@
   </si>
   <si>
     <t>Total Companies</t>
+  </si>
+  <si>
+    <t>Country Name</t>
+  </si>
+  <si>
+    <t>Grenada</t>
+  </si>
+  <si>
+    <t>Jamaica</t>
+  </si>
+  <si>
+    <t>Togo</t>
+  </si>
+  <si>
+    <t>Sao Tome and Principe</t>
+  </si>
+  <si>
+    <t>Bermuda</t>
+  </si>
+  <si>
+    <t>Mauritius</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Republic of the Congo</t>
+  </si>
+  <si>
+    <t>Ethiopa</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>Oman</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Phillippines</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>Luxembourg</t>
+  </si>
+  <si>
+    <t>Djibouti</t>
+  </si>
+  <si>
+    <t>Seychelles</t>
+  </si>
+  <si>
+    <t>Saint Martin</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Jersey</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Tonga</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>Liberia</t>
+  </si>
+  <si>
+    <t>Sierra Leone</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>Armenia</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Mali</t>
+  </si>
+  <si>
+    <t>Cayman Islands</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
+  </si>
+  <si>
+    <t>South Korea</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>Gibraltar</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Montenegro</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -683,16 +865,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1025,7 +1210,7 @@
   <dimension ref="A1:B214"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3167,490 +3352,846 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B151"/>
+  <dimension ref="A1:D151"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>199</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>183</v>
       </c>
       <c r="B2" s="1">
         <v>750000000</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D2" s="2">
+        <v>107818</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>173</v>
       </c>
       <c r="B3" s="1">
         <v>416694000</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2847232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>97</v>
       </c>
       <c r="B4" s="1">
         <v>407800000</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D4" s="2">
+        <v>6587239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>106</v>
       </c>
       <c r="B5" s="1">
         <v>165000000</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="2">
+        <v>175808</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>196</v>
       </c>
       <c r="B6" s="1">
         <v>132451682.76922999</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" s="2">
+        <v>65365</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>115</v>
       </c>
       <c r="B7" s="1">
         <v>119476217.571428</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1294104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>152</v>
       </c>
       <c r="B8" s="1">
         <v>111405512.59675699</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" t="s">
+        <v>210</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1330044000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>177</v>
       </c>
       <c r="B9" s="1">
         <v>105000000</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" t="s">
+        <v>211</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3039126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>87</v>
       </c>
       <c r="B10" s="1">
         <v>103717400</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" t="s">
+        <v>212</v>
+      </c>
+      <c r="D10" s="2">
+        <v>88013491</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>86</v>
       </c>
       <c r="B11" s="1">
         <v>103091000</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11" t="s">
+        <v>213</v>
+      </c>
+      <c r="D11" s="2">
+        <v>840926</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>51</v>
       </c>
       <c r="B12" s="1">
         <v>64103536.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12" t="s">
+        <v>214</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2967717</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>98</v>
       </c>
       <c r="B13" s="1">
         <v>58892604.646258503</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" t="s">
+        <v>215</v>
+      </c>
+      <c r="D13" s="2">
+        <v>49000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>59</v>
       </c>
       <c r="B14" s="1">
         <v>43629950.765432097</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14" t="s">
+        <v>216</v>
+      </c>
+      <c r="D14" s="2">
+        <v>99900177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>94</v>
       </c>
       <c r="B15" s="1">
         <v>43088323.454545401</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D15" s="2">
+        <v>40046566</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>60</v>
       </c>
       <c r="B16" s="1">
         <v>41046143.032128498</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" t="s">
+        <v>218</v>
+      </c>
+      <c r="D16" s="2">
+        <v>127288000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>144</v>
       </c>
       <c r="B17" s="1">
         <v>40592769.599653304</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" t="s">
+        <v>219</v>
+      </c>
+      <c r="D17" s="2">
+        <v>140702000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>188</v>
       </c>
       <c r="B18" s="1">
         <v>39893826.375</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" t="s">
+        <v>220</v>
+      </c>
+      <c r="D18" s="2">
+        <v>76923000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>104</v>
       </c>
       <c r="B19" s="1">
         <v>36071059.448275797</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" t="s">
+        <v>221</v>
+      </c>
+      <c r="D19" s="2">
+        <v>242968342</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>171</v>
       </c>
       <c r="B20" s="1">
         <v>33256525.443708599</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" t="s">
+        <v>223</v>
+      </c>
+      <c r="D20" s="2">
+        <v>4975593</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>119</v>
       </c>
       <c r="B21" s="1">
         <v>30746395.2558139</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" t="s">
+        <v>224</v>
+      </c>
+      <c r="D21" s="2">
+        <v>497538</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>52</v>
       </c>
       <c r="B22" s="1">
         <v>30000000</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" t="s">
+        <v>225</v>
+      </c>
+      <c r="D22" s="2">
+        <v>740528</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>178</v>
       </c>
       <c r="B23" s="1">
         <v>29458968.734966502</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" t="s">
+        <v>226</v>
+      </c>
+      <c r="D23" s="2">
+        <v>88340</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>160</v>
       </c>
       <c r="B24" s="1">
         <v>29243184</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" t="s">
+        <v>227</v>
+      </c>
+      <c r="D24" s="2">
+        <v>35295</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>58</v>
       </c>
       <c r="B25" s="1">
         <v>28900000</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" t="s">
+        <v>228</v>
+      </c>
+      <c r="D25" s="2">
+        <v>21281844</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>151</v>
       </c>
       <c r="B26" s="1">
         <v>27689406</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26" t="s">
+        <v>229</v>
+      </c>
+      <c r="D26" s="2">
+        <v>34586184</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>121</v>
       </c>
       <c r="B27" s="1">
         <v>24588596.449462298</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" t="s">
+        <v>230</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1173108018</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>154</v>
       </c>
       <c r="B28" s="1">
         <v>24381727.666666601</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" t="s">
+        <v>231</v>
+      </c>
+      <c r="D28" s="2">
+        <v>90812</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>122</v>
       </c>
       <c r="B29" s="1">
         <v>24024777.584026601</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" t="s">
+        <v>232</v>
+      </c>
+      <c r="D29" s="2">
+        <v>4701069</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>61</v>
       </c>
       <c r="B30" s="1">
         <v>23360010.526785702</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30" t="s">
+        <v>233</v>
+      </c>
+      <c r="D30" s="2">
+        <v>122580</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>146</v>
       </c>
       <c r="B31" s="1">
         <v>23304588.214711599</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31" t="s">
+        <v>234</v>
+      </c>
+      <c r="D31" s="2">
+        <v>310232863</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>159</v>
       </c>
       <c r="B32" s="1">
         <v>20000000</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" t="s">
+        <v>235</v>
+      </c>
+      <c r="D32" s="2">
+        <v>3685076</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>161</v>
       </c>
       <c r="B33" s="1">
         <v>20000000</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" t="s">
+        <v>236</v>
+      </c>
+      <c r="D33" s="2">
+        <v>5245695</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>80</v>
       </c>
       <c r="B34" s="1">
         <v>19101748.6173633</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34" t="s">
+        <v>237</v>
+      </c>
+      <c r="D34" s="2">
+        <v>6898686</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>70</v>
       </c>
       <c r="B35" s="1">
         <v>18664694.833333299</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" t="s">
+        <v>238</v>
+      </c>
+      <c r="D35" s="2">
+        <v>2968000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>54</v>
       </c>
       <c r="B36" s="1">
         <v>17984460.597266801</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36" t="s">
+        <v>239</v>
+      </c>
+      <c r="D36" s="2">
+        <v>81802257</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>120</v>
       </c>
       <c r="B37" s="1">
         <v>17614584.059523799</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37" t="s">
+        <v>240</v>
+      </c>
+      <c r="D37" s="2">
+        <v>67089500</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>124</v>
       </c>
       <c r="B38" s="1">
         <v>17585481</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38" t="s">
+        <v>241</v>
+      </c>
+      <c r="D38" s="2">
+        <v>13796354</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>129</v>
       </c>
       <c r="B39" s="1">
         <v>17043109.2352941</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39" t="s">
+        <v>242</v>
+      </c>
+      <c r="D39" s="2">
+        <v>44270</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>110</v>
       </c>
       <c r="B40" s="1">
         <v>16574187.5304347</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40" t="s">
+        <v>243</v>
+      </c>
+      <c r="D40" s="2">
+        <v>38500000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>182</v>
       </c>
       <c r="B41" s="1">
         <v>15390333.3333333</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="C41" t="s">
+        <v>244</v>
+      </c>
+      <c r="D41" s="2">
+        <v>11651858</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>53</v>
       </c>
       <c r="B42" s="1">
         <v>14860726.447396301</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="C42" t="s">
+        <v>245</v>
+      </c>
+      <c r="D42" s="2">
+        <v>46505963</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>107</v>
       </c>
       <c r="B43" s="1">
         <v>14635196.8571428</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43" t="s">
+        <v>246</v>
+      </c>
+      <c r="D43" s="2">
+        <v>89571130</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>132</v>
       </c>
       <c r="B44" s="1">
         <v>14301231.7876823</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="C44" t="s">
+        <v>247</v>
+      </c>
+      <c r="D44" s="2">
+        <v>16654000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>170</v>
       </c>
       <c r="B45" s="1">
         <v>14117805.594890499</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="C45" t="s">
+        <v>248</v>
+      </c>
+      <c r="D45" s="2">
+        <v>4622917</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>101</v>
       </c>
       <c r="B46" s="1">
         <v>14101891.3571428</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="C46" t="s">
+        <v>249</v>
+      </c>
+      <c r="D46" s="2">
+        <v>22894384</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>134</v>
       </c>
       <c r="B47" s="1">
         <v>13446969.6743697</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="C47" t="s">
+        <v>250</v>
+      </c>
+      <c r="D47" s="2">
+        <v>48422644</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>167</v>
       </c>
       <c r="B48" s="1">
         <v>13343116.2127659</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="C48" t="s">
+        <v>251</v>
+      </c>
+      <c r="D48" s="2">
+        <v>4252277</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>126</v>
       </c>
       <c r="B49" s="1">
         <v>13324539.639256099</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="C49" t="s">
+        <v>252</v>
+      </c>
+      <c r="D49" s="2">
+        <v>33679000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>75</v>
       </c>
       <c r="B50" s="1">
         <v>13051112.515297901</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="C50" t="s">
+        <v>253</v>
+      </c>
+      <c r="D50" s="2">
+        <v>7353985</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>92</v>
       </c>
       <c r="B51" s="1">
         <v>12814700.3472222</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="C51" t="s">
+        <v>254</v>
+      </c>
+      <c r="D51" s="2">
+        <v>80471869</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>191</v>
       </c>
       <c r="B52" s="1">
         <v>12550898.5</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="C52" t="s">
+        <v>255</v>
+      </c>
+      <c r="D52" s="2">
+        <v>27884</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>147</v>
       </c>
       <c r="B53" s="1">
         <v>12432057.826315699</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="C53" t="s">
+        <v>256</v>
+      </c>
+      <c r="D53" s="2">
+        <v>5009150</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>184</v>
       </c>
       <c r="B54" s="1">
         <v>12407827.792922599</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="C54" t="s">
+        <v>257</v>
+      </c>
+      <c r="D54" s="2">
+        <v>9555893</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>138</v>
       </c>
       <c r="B55" s="1">
         <v>12292790.585142801</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="C55" t="s">
+        <v>258</v>
+      </c>
+      <c r="D55" s="2">
+        <v>21515754</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>67</v>
       </c>
       <c r="B56" s="1">
         <v>12200000</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="C56" t="s">
+        <v>259</v>
+      </c>
+      <c r="D56" s="2">
+        <v>666730</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>186</v>
       </c>
       <c r="B57" s="1">
         <v>12150381.671145201</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="C57" t="s">
+        <v>260</v>
+      </c>
+      <c r="D57" s="2">
+        <v>64768389</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>142</v>
       </c>
       <c r="B58" s="1">
         <v>11890074.0283185</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="C58" t="s">
+        <v>261</v>
+      </c>
+      <c r="D58" s="2">
+        <v>201103330</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>116</v>
       </c>
       <c r="B59" s="1">
         <v>11812811.6734656</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="C59" t="s">
+        <v>262</v>
+      </c>
+      <c r="D59" s="2">
+        <v>62348447</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>50</v>
       </c>
@@ -3658,7 +4199,7 @@
         <v>11673640.4666666</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
         <v>150</v>
       </c>
@@ -3666,7 +4207,7 @@
         <v>11632458.9054054</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
         <v>156</v>
       </c>
@@ -3674,7 +4215,7 @@
         <v>11554262</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
         <v>69</v>
       </c>
@@ -3682,7 +4223,7 @@
         <v>10255713.430232501</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
         <v>139</v>
       </c>
@@ -4387,11 +4928,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B151">
-    <sortState ref="A2:B151">
-      <sortCondition descending="1" ref="B1:B151"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:D151"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -7379,7 +7916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Finished filling in country names/population data
</commit_message>
<xml_diff>
--- a/startup_analysis.xlsx
+++ b/startup_analysis.xlsx
@@ -19,7 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Avg_funding_cat!$A$1:$B$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Avg_funding_country!$A$1:$D$151</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Companies_per_category!$A$1:$B$47</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Country_count!$A$1:$B$151</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Country_count!$A$1:$D$151</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Num_founded_per_year!$A$1:$B$214</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="355">
   <si>
     <t>Year</t>
   </si>
@@ -821,6 +821,282 @@
   </si>
   <si>
     <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Honduras</t>
+  </si>
+  <si>
+    <t>Iraq</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Democratic Republic of the Congo</t>
+  </si>
+  <si>
+    <t>Columbia</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Ivory Coast</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
+    <t>Barbados</t>
+  </si>
+  <si>
+    <t>Moldova</t>
+  </si>
+  <si>
+    <t>Bosnia and Herzegovina</t>
+  </si>
+  <si>
+    <t>Reunion</t>
+  </si>
+  <si>
+    <t>Uzbekistan</t>
+  </si>
+  <si>
+    <t>Dominica</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>Dominican Republic</t>
+  </si>
+  <si>
+    <t>North Korea</t>
+  </si>
+  <si>
+    <t>Ecuador</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>Isle of Man</t>
+  </si>
+  <si>
+    <t>Liechtenstein</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>Macedonia</t>
+  </si>
+  <si>
+    <t>Monaco</t>
+  </si>
+  <si>
+    <t>El Salvador</t>
+  </si>
+  <si>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>Azerbaijan</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Nicaragua</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
+  </si>
+  <si>
+    <t>Belarus</t>
+  </si>
+  <si>
+    <t>Botswana</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>Belize</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Myanmar</t>
+  </si>
+  <si>
+    <t>Martinique</t>
+  </si>
+  <si>
+    <t>Tanzania</t>
+  </si>
+  <si>
+    <t>Cyprus</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Uganda</t>
+  </si>
+  <si>
+    <t>Tunisia</t>
+  </si>
+  <si>
+    <t>Guernsey</t>
+  </si>
+  <si>
+    <t>Kuwait</t>
+  </si>
+  <si>
+    <t>Paraguay</t>
+  </si>
+  <si>
+    <t>Bahamas</t>
+  </si>
+  <si>
+    <t>Trinidad and Tobago</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Lithuania</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Haiti</t>
+  </si>
+  <si>
+    <t>Palestine</t>
+  </si>
+  <si>
+    <t>Malta</t>
+  </si>
+  <si>
+    <t>Laos</t>
+  </si>
+  <si>
+    <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>Somalia</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Panama</t>
+  </si>
+  <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>Nepal</t>
   </si>
 </sst>
 </file>
@@ -832,7 +1108,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -843,6 +1119,22 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -865,19 +1157,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3361,7 +3665,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3681,10 +3985,10 @@
         <v>29458968.734966502</v>
       </c>
       <c r="C23" t="s">
-        <v>226</v>
+        <v>287</v>
       </c>
       <c r="D23" s="2">
-        <v>88340</v>
+        <v>7581000</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -4198,6 +4502,12 @@
       <c r="B60" s="1">
         <v>11673640.4666666</v>
       </c>
+      <c r="C60" t="s">
+        <v>325</v>
+      </c>
+      <c r="D60" s="2">
+        <v>41892895</v>
+      </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
@@ -4206,6 +4516,12 @@
       <c r="B61" s="1">
         <v>11632458.9054054</v>
       </c>
+      <c r="C61" t="s">
+        <v>265</v>
+      </c>
+      <c r="D61" s="2">
+        <v>28274729</v>
+      </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
@@ -4214,6 +4530,12 @@
       <c r="B62" s="1">
         <v>11554262</v>
       </c>
+      <c r="C62" t="s">
+        <v>266</v>
+      </c>
+      <c r="D62" s="2">
+        <v>70916439</v>
+      </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
@@ -4222,6 +4544,12 @@
       <c r="B63" s="1">
         <v>10255713.430232501</v>
       </c>
+      <c r="C63" t="s">
+        <v>267</v>
+      </c>
+      <c r="D63" s="2">
+        <v>47790000</v>
+      </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
@@ -4230,706 +4558,1239 @@
       <c r="B64" s="1">
         <v>8388756.3333333302</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
+      <c r="C64" t="s">
+        <v>268</v>
+      </c>
+      <c r="D64" s="2">
+        <v>738004</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>155</v>
       </c>
       <c r="B65" s="1">
         <v>8179889.1049382696</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
+      <c r="C65" t="s">
+        <v>269</v>
+      </c>
+      <c r="D65" s="2">
+        <v>8205000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>93</v>
       </c>
       <c r="B66" s="1">
         <v>7592461.4800000004</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
+      <c r="C66" t="s">
+        <v>270</v>
+      </c>
+      <c r="D66" s="2">
+        <v>5484000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>78</v>
       </c>
       <c r="B67" s="1">
         <v>7543402.5794701902</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
+      <c r="C67" t="s">
+        <v>271</v>
+      </c>
+      <c r="D67" s="2">
+        <v>10403000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>149</v>
       </c>
       <c r="B68" s="1">
         <v>6862851.7605633801</v>
       </c>
-    </row>
-    <row r="69" spans="1:2">
+      <c r="C68" t="s">
+        <v>272</v>
+      </c>
+      <c r="D68" s="2">
+        <v>2217969</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
         <v>95</v>
       </c>
       <c r="B69" s="1">
         <v>6621503.3053097297</v>
       </c>
-    </row>
-    <row r="70" spans="1:2">
+      <c r="C69" t="s">
+        <v>273</v>
+      </c>
+      <c r="D69" s="2">
+        <v>112468855</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>103</v>
       </c>
       <c r="B70" s="1">
         <v>6547546.1666666605</v>
       </c>
-    </row>
-    <row r="71" spans="1:2">
+      <c r="C70" t="s">
+        <v>274</v>
+      </c>
+      <c r="D70" s="2">
+        <v>21058798</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
         <v>141</v>
       </c>
       <c r="B71" s="1">
         <v>6471294.9756097496</v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
+      <c r="C71" t="s">
+        <v>275</v>
+      </c>
+      <c r="D71" s="2">
+        <v>184404791</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
         <v>123</v>
       </c>
       <c r="B72" s="1">
         <v>5531039.3578947298</v>
       </c>
-    </row>
-    <row r="73" spans="1:2">
+      <c r="C72" t="s">
+        <v>276</v>
+      </c>
+      <c r="D72" s="2">
+        <v>10476000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>135</v>
       </c>
       <c r="B73" s="1">
         <v>5500000</v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
+      <c r="C73" t="s">
+        <v>277</v>
+      </c>
+      <c r="D73" s="2">
+        <v>286653</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>190</v>
       </c>
       <c r="B74" s="1">
         <v>5301937.2623376604</v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
+      <c r="C74" t="s">
+        <v>288</v>
+      </c>
+      <c r="D74" s="2">
+        <v>5244000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>49</v>
       </c>
       <c r="B75" s="1">
         <v>5000000</v>
       </c>
-    </row>
-    <row r="76" spans="1:2">
+      <c r="C75" t="s">
+        <v>289</v>
+      </c>
+      <c r="D75" s="2">
+        <v>75049</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>172</v>
       </c>
       <c r="B76" s="1">
         <v>4453268</v>
       </c>
-    </row>
-    <row r="77" spans="1:2">
+      <c r="C76" t="s">
+        <v>290</v>
+      </c>
+      <c r="D76" s="2">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
         <v>96</v>
       </c>
       <c r="B77" s="1">
         <v>4339423.3809523797</v>
       </c>
-    </row>
-    <row r="78" spans="1:2">
+      <c r="C77" t="s">
+        <v>291</v>
+      </c>
+      <c r="D77" s="2">
+        <v>156118464</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
         <v>85</v>
       </c>
       <c r="B78" s="1">
         <v>4157476.74953959</v>
       </c>
-    </row>
-    <row r="79" spans="1:2">
+      <c r="C78" t="s">
+        <v>292</v>
+      </c>
+      <c r="D78" s="2">
+        <v>60340328</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
         <v>137</v>
       </c>
       <c r="B79" s="1">
         <v>4084241.7286432101</v>
       </c>
-    </row>
-    <row r="80" spans="1:2">
+      <c r="C79" t="s">
+        <v>293</v>
+      </c>
+      <c r="D79" s="2">
+        <v>77804122</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
         <v>81</v>
       </c>
       <c r="B80" s="1">
         <v>3951346.2222222202</v>
       </c>
-    </row>
-    <row r="81" spans="1:2">
+      <c r="C80" t="s">
+        <v>326</v>
+      </c>
+      <c r="D80" s="2">
+        <v>1102677</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81" t="s">
         <v>163</v>
       </c>
       <c r="B81" s="1">
         <v>3622853.81818181</v>
       </c>
-    </row>
-    <row r="82" spans="1:2">
+      <c r="C81" t="s">
+        <v>327</v>
+      </c>
+      <c r="D81" s="2">
+        <v>11000000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82" t="s">
         <v>100</v>
       </c>
       <c r="B82" s="1">
         <v>3612972</v>
       </c>
-    </row>
-    <row r="83" spans="1:2">
+      <c r="C82" t="s">
+        <v>328</v>
+      </c>
+      <c r="D82" s="2">
+        <v>12323252</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" t="s">
         <v>118</v>
       </c>
       <c r="B83" s="1">
         <v>3543425.31578947</v>
       </c>
-    </row>
-    <row r="84" spans="1:2">
+      <c r="C83" t="s">
+        <v>329</v>
+      </c>
+      <c r="D83" s="2">
+        <v>33398682</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84" t="s">
         <v>174</v>
       </c>
       <c r="B84" s="1">
         <v>3535354</v>
       </c>
-    </row>
-    <row r="85" spans="1:2">
+      <c r="C84" t="s">
+        <v>330</v>
+      </c>
+      <c r="D84" s="2">
+        <v>10589025</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85" t="s">
         <v>179</v>
       </c>
       <c r="B85" s="1">
         <v>3480000</v>
       </c>
-    </row>
-    <row r="86" spans="1:2">
+      <c r="C85" t="s">
+        <v>331</v>
+      </c>
+      <c r="D85" s="2">
+        <v>65228</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86" t="s">
         <v>57</v>
       </c>
       <c r="B86" s="1">
         <v>3442666.6</v>
       </c>
-    </row>
-    <row r="87" spans="1:2">
+      <c r="C86" t="s">
+        <v>332</v>
+      </c>
+      <c r="D86" s="2">
+        <v>2789132</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87" t="s">
         <v>169</v>
       </c>
       <c r="B87" s="1">
         <v>3412500</v>
       </c>
-    </row>
-    <row r="88" spans="1:2">
+      <c r="C87" t="s">
+        <v>333</v>
+      </c>
+      <c r="D87" s="2">
+        <v>6375830</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88" t="s">
         <v>72</v>
       </c>
       <c r="B88" s="1">
         <v>3386666.66666666</v>
       </c>
-    </row>
-    <row r="89" spans="1:2">
+      <c r="C88" t="s">
+        <v>334</v>
+      </c>
+      <c r="D88" s="2">
+        <v>301790</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89" t="s">
         <v>185</v>
       </c>
       <c r="B89" s="1">
         <v>3378857.1428571399</v>
       </c>
-    </row>
-    <row r="90" spans="1:2">
+      <c r="C89" t="s">
+        <v>335</v>
+      </c>
+      <c r="D89" s="2">
+        <v>1228691</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90" t="s">
         <v>157</v>
       </c>
       <c r="B90" s="1">
         <v>3232290.57142857</v>
       </c>
-    </row>
-    <row r="91" spans="1:2">
+      <c r="C90" t="s">
+        <v>336</v>
+      </c>
+      <c r="D90" s="2">
+        <v>13550440</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91" t="s">
         <v>76</v>
       </c>
       <c r="B91" s="1">
         <v>3115011.56164383</v>
       </c>
-    </row>
-    <row r="92" spans="1:2">
+      <c r="C91" t="s">
+        <v>337</v>
+      </c>
+      <c r="D91" s="2">
+        <v>41343201</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92" t="s">
         <v>83</v>
       </c>
       <c r="B92" s="1">
         <v>3091123.375</v>
       </c>
-    </row>
-    <row r="93" spans="1:2">
+      <c r="C92" t="s">
+        <v>338</v>
+      </c>
+      <c r="D92" s="2">
+        <v>31627428</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
       <c r="A93" t="s">
         <v>140</v>
       </c>
       <c r="B93" s="1">
         <v>2908937.9117647</v>
       </c>
-    </row>
-    <row r="94" spans="1:2">
+      <c r="C93" t="s">
+        <v>339</v>
+      </c>
+      <c r="D93" s="2">
+        <v>6407085</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
       <c r="A94" t="s">
         <v>166</v>
       </c>
       <c r="B94" s="1">
         <v>2754292.5932203298</v>
       </c>
-    </row>
-    <row r="95" spans="1:2">
+      <c r="C94" t="s">
+        <v>340</v>
+      </c>
+      <c r="D94" s="2">
+        <v>2944459</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95" t="s">
         <v>111</v>
       </c>
       <c r="B95" s="1">
         <v>2561481.5</v>
       </c>
-    </row>
-    <row r="96" spans="1:2">
+      <c r="C95" t="s">
+        <v>341</v>
+      </c>
+      <c r="D95" s="2">
+        <v>2986952</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96" t="s">
         <v>71</v>
       </c>
       <c r="B96" s="1">
         <v>2541939.8888888801</v>
       </c>
-    </row>
-    <row r="97" spans="1:2">
+      <c r="C96" t="s">
+        <v>342</v>
+      </c>
+      <c r="D96" s="2">
+        <v>21513990</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97" t="s">
         <v>181</v>
       </c>
       <c r="B97" s="1">
         <v>2507253.8095237999</v>
       </c>
-    </row>
-    <row r="98" spans="1:2">
+      <c r="C97" t="s">
+        <v>343</v>
+      </c>
+      <c r="D97" s="2">
+        <v>24339838</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
         <v>82</v>
       </c>
       <c r="B98" s="1">
         <v>2500000</v>
       </c>
-    </row>
-    <row r="99" spans="1:2">
+      <c r="C98" t="s">
+        <v>344</v>
+      </c>
+      <c r="D98" s="2">
+        <v>96489245</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
         <v>180</v>
       </c>
       <c r="B99" s="1">
         <v>2380000</v>
       </c>
-    </row>
-    <row r="100" spans="1:2">
+      <c r="C99" t="s">
+        <v>345</v>
+      </c>
+      <c r="D99" s="2">
+        <v>3800000</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100" t="s">
         <v>148</v>
       </c>
       <c r="B100" s="1">
         <v>2207659.3333333302</v>
       </c>
-    </row>
-    <row r="101" spans="1:2">
+      <c r="C100" t="s">
+        <v>346</v>
+      </c>
+      <c r="D100" s="2">
+        <v>403000</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101" t="s">
         <v>164</v>
       </c>
       <c r="B101" s="1">
         <v>2100000</v>
       </c>
-    </row>
-    <row r="102" spans="1:2">
+      <c r="C101" t="s">
+        <v>347</v>
+      </c>
+      <c r="D101" s="2">
+        <v>6368162</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
       <c r="A102" t="s">
         <v>125</v>
       </c>
       <c r="B102" s="1">
         <v>2080985.8571428501</v>
       </c>
-    </row>
-    <row r="103" spans="1:2">
+      <c r="C102" t="s">
+        <v>348</v>
+      </c>
+      <c r="D102" s="2">
+        <v>3916632</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
       <c r="A103" t="s">
         <v>128</v>
       </c>
       <c r="B103" s="1">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="104" spans="1:2">
+      <c r="C103" t="s">
+        <v>349</v>
+      </c>
+      <c r="D103" s="2">
+        <v>10112453</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
       <c r="A104" t="s">
         <v>153</v>
       </c>
       <c r="B104" s="1">
         <v>1918796.8731343199</v>
       </c>
-    </row>
-    <row r="105" spans="1:2">
+      <c r="C104" t="s">
+        <v>350</v>
+      </c>
+      <c r="D104" s="2">
+        <v>10676000</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
       <c r="A105" t="s">
         <v>74</v>
       </c>
       <c r="B105" s="1">
         <v>1869841.7857142801</v>
       </c>
-    </row>
-    <row r="106" spans="1:2">
+      <c r="C105" t="s">
+        <v>351</v>
+      </c>
+      <c r="D105" s="2">
+        <v>3410676</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
       <c r="A106" t="s">
         <v>79</v>
       </c>
       <c r="B106" s="1">
         <v>1777632.9482758599</v>
       </c>
-    </row>
-    <row r="107" spans="1:2">
+      <c r="C106" t="s">
+        <v>352</v>
+      </c>
+      <c r="D106" s="2">
+        <v>29907003</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
       <c r="A107" t="s">
         <v>64</v>
       </c>
       <c r="B107" s="1">
         <v>1607614.61788617</v>
       </c>
-    </row>
-    <row r="108" spans="1:2">
+      <c r="C107" t="s">
+        <v>353</v>
+      </c>
+      <c r="D107" s="2">
+        <v>1291170</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
       <c r="A108" t="s">
         <v>62</v>
       </c>
       <c r="B108" s="1">
         <v>1507623.1428571399</v>
       </c>
-    </row>
-    <row r="109" spans="1:2">
+      <c r="C108" t="s">
+        <v>354</v>
+      </c>
+      <c r="D108" s="2">
+        <v>28951852</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
       <c r="A109" t="s">
         <v>189</v>
       </c>
       <c r="B109" s="1">
         <v>1501137.5131578899</v>
       </c>
-    </row>
-    <row r="110" spans="1:2">
+      <c r="C109" t="s">
+        <v>317</v>
+      </c>
+      <c r="D109" s="2">
+        <v>9932000</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
       <c r="A110" t="s">
         <v>158</v>
       </c>
       <c r="B110" s="1">
         <v>1490000</v>
       </c>
-    </row>
-    <row r="111" spans="1:2">
+      <c r="C110" t="s">
+        <v>324</v>
+      </c>
+      <c r="D110" s="2">
+        <v>386486</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
       <c r="A111" t="s">
         <v>90</v>
       </c>
       <c r="B111" s="1">
         <v>1454634.4</v>
       </c>
-    </row>
-    <row r="112" spans="1:2">
+      <c r="C111" t="s">
+        <v>318</v>
+      </c>
+      <c r="D111" s="2">
+        <v>3477000</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
       <c r="A112" t="s">
         <v>117</v>
       </c>
       <c r="B112" s="1">
         <v>1430773.3076923001</v>
       </c>
-    </row>
-    <row r="113" spans="1:2">
+      <c r="C112" t="s">
+        <v>319</v>
+      </c>
+      <c r="D112" s="2">
+        <v>21959278</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
       <c r="A113" t="s">
         <v>108</v>
       </c>
       <c r="B113" s="1">
         <v>1409824.0263157799</v>
       </c>
-    </row>
-    <row r="114" spans="1:2">
+      <c r="C113" t="s">
+        <v>320</v>
+      </c>
+      <c r="D113" s="2">
+        <v>5455000</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
       <c r="A114" t="s">
         <v>187</v>
       </c>
       <c r="B114" s="1">
         <v>1371913.6954314699</v>
       </c>
-    </row>
-    <row r="115" spans="1:2">
+      <c r="C114" t="s">
+        <v>321</v>
+      </c>
+      <c r="D114" s="2">
+        <v>308910</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
       <c r="A115" t="s">
         <v>114</v>
       </c>
       <c r="B115" s="1">
         <v>1287861.1111111101</v>
       </c>
-    </row>
-    <row r="116" spans="1:2">
+      <c r="C115" t="s">
+        <v>322</v>
+      </c>
+      <c r="D115" s="2">
+        <v>4125247</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
       <c r="A116" t="s">
         <v>197</v>
       </c>
       <c r="B116" s="1">
         <v>1237783.83333333</v>
       </c>
-    </row>
-    <row r="117" spans="1:2">
+      <c r="C116" t="s">
+        <v>323</v>
+      </c>
+      <c r="D116" s="2">
+        <v>53414374</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
       <c r="A117" t="s">
         <v>127</v>
       </c>
       <c r="B117" s="1">
         <v>1181314.5546218399</v>
       </c>
-    </row>
-    <row r="118" spans="1:2">
+      <c r="C117" t="s">
+        <v>294</v>
+      </c>
+      <c r="D117" s="2">
+        <v>45415596</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
       <c r="A118" t="s">
         <v>192</v>
       </c>
       <c r="B118" s="1">
         <v>1145279</v>
       </c>
-    </row>
-    <row r="119" spans="1:2">
+      <c r="C118" t="s">
+        <v>295</v>
+      </c>
+      <c r="D118" s="2">
+        <v>25731776</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
       <c r="A119" t="s">
         <v>112</v>
       </c>
       <c r="B119" s="1">
         <v>783447.02439024299</v>
       </c>
-    </row>
-    <row r="120" spans="1:2">
+      <c r="C119" t="s">
+        <v>296</v>
+      </c>
+      <c r="D119" s="2">
+        <v>2007000</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
       <c r="A120" t="s">
         <v>84</v>
       </c>
       <c r="B120" s="1">
         <v>742498.6</v>
       </c>
-    </row>
-    <row r="121" spans="1:2">
+      <c r="C120" t="s">
+        <v>297</v>
+      </c>
+      <c r="D120" s="2">
+        <v>11055976</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
       <c r="A121" t="s">
         <v>133</v>
       </c>
       <c r="B121" s="1">
         <v>663613.66666666605</v>
       </c>
-    </row>
-    <row r="122" spans="1:2">
+      <c r="C121" t="s">
+        <v>298</v>
+      </c>
+      <c r="D121" s="2">
+        <v>2062294</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
       <c r="A122" t="s">
         <v>130</v>
       </c>
       <c r="B122" s="1">
         <v>658290.33333333302</v>
       </c>
-    </row>
-    <row r="123" spans="1:2">
+      <c r="C122" t="s">
+        <v>299</v>
+      </c>
+      <c r="D122" s="2">
+        <v>32965</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
       <c r="A123" t="s">
         <v>198</v>
       </c>
       <c r="B123" s="1">
         <v>616666.66666666605</v>
       </c>
-    </row>
-    <row r="124" spans="1:2">
+      <c r="C123" t="s">
+        <v>300</v>
+      </c>
+      <c r="D123" s="2">
+        <v>6052064</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
       <c r="A124" t="s">
         <v>143</v>
       </c>
       <c r="B124" s="1">
         <v>561854.875</v>
       </c>
-    </row>
-    <row r="125" spans="1:2">
+      <c r="C124" t="s">
+        <v>301</v>
+      </c>
+      <c r="D124" s="2">
+        <v>4491000</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
       <c r="A125" t="s">
         <v>195</v>
       </c>
       <c r="B125" s="1">
         <v>542142.85714285704</v>
       </c>
-    </row>
-    <row r="126" spans="1:2">
+      <c r="C125" t="s">
+        <v>302</v>
+      </c>
+      <c r="D125" s="2">
+        <v>14453680</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
       <c r="A126" t="s">
         <v>73</v>
       </c>
       <c r="B126" s="1">
         <v>527998.76923076902</v>
       </c>
-    </row>
-    <row r="127" spans="1:2">
+      <c r="C126" t="s">
+        <v>303</v>
+      </c>
+      <c r="D126" s="2">
+        <v>8303512</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
       <c r="A127" t="s">
         <v>168</v>
       </c>
       <c r="B127" s="1">
         <v>515246.09090909001</v>
       </c>
-    </row>
-    <row r="128" spans="1:2">
+      <c r="C127" t="s">
+        <v>304</v>
+      </c>
+      <c r="D127" s="2">
+        <v>7148785</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
       <c r="A128" t="s">
         <v>55</v>
       </c>
       <c r="B128" s="1">
         <v>475000</v>
       </c>
-    </row>
-    <row r="129" spans="1:2">
+      <c r="C128" t="s">
+        <v>305</v>
+      </c>
+      <c r="D128" s="2">
+        <v>5995928</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
       <c r="A129" t="s">
         <v>165</v>
       </c>
       <c r="B129" s="1">
         <v>464322.14285714203</v>
       </c>
-    </row>
-    <row r="130" spans="1:2">
+      <c r="C129" t="s">
+        <v>306</v>
+      </c>
+      <c r="D129" s="2">
+        <v>4516220</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
       <c r="A130" t="s">
         <v>89</v>
       </c>
       <c r="B130" s="1">
         <v>403431.78260869498</v>
       </c>
-    </row>
-    <row r="131" spans="1:2">
+      <c r="C130" t="s">
+        <v>307</v>
+      </c>
+      <c r="D130" s="2">
+        <v>7344847</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
       <c r="A131" t="s">
         <v>136</v>
       </c>
       <c r="B131" s="1">
         <v>403333.33333333302</v>
       </c>
-    </row>
-    <row r="132" spans="1:2">
+      <c r="C131" t="s">
+        <v>308</v>
+      </c>
+      <c r="D131" s="2">
+        <v>15340000</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
       <c r="A132" t="s">
         <v>194</v>
       </c>
       <c r="B132" s="1">
         <v>399545.45454545401</v>
       </c>
-    </row>
-    <row r="133" spans="1:2">
+      <c r="C132" t="s">
+        <v>309</v>
+      </c>
+      <c r="D132" s="2">
+        <v>9685000</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
       <c r="A133" t="s">
         <v>68</v>
       </c>
       <c r="B133" s="1">
         <v>375500</v>
       </c>
-    </row>
-    <row r="134" spans="1:2">
+      <c r="C133" t="s">
+        <v>310</v>
+      </c>
+      <c r="D133" s="2">
+        <v>2029307</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
       <c r="A134" t="s">
         <v>77</v>
       </c>
       <c r="B134" s="1">
         <v>369352.51436781598</v>
       </c>
-    </row>
-    <row r="135" spans="1:2">
+      <c r="C134" t="s">
+        <v>311</v>
+      </c>
+      <c r="D134" s="2">
+        <v>16746491</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
       <c r="A135" t="s">
         <v>63</v>
       </c>
       <c r="B135" s="1">
         <v>350000</v>
       </c>
-    </row>
-    <row r="136" spans="1:2">
+      <c r="C135" t="s">
+        <v>312</v>
+      </c>
+      <c r="D135" s="2">
+        <v>22061451</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
       <c r="A136" t="s">
         <v>193</v>
       </c>
       <c r="B136" s="1">
         <v>304411.2</v>
       </c>
-    </row>
-    <row r="137" spans="1:2">
+      <c r="C136" t="s">
+        <v>313</v>
+      </c>
+      <c r="D136" s="2">
+        <v>13460305</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
       <c r="A137" t="s">
         <v>102</v>
       </c>
       <c r="B137" s="1">
         <v>265721</v>
       </c>
-    </row>
-    <row r="138" spans="1:2">
+      <c r="C137" t="s">
+        <v>314</v>
+      </c>
+      <c r="D137" s="2">
+        <v>314522</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
       <c r="A138" t="s">
         <v>56</v>
       </c>
       <c r="B138" s="1">
         <v>258473.9</v>
       </c>
-    </row>
-    <row r="139" spans="1:2">
+      <c r="C138" t="s">
+        <v>315</v>
+      </c>
+      <c r="D138" s="2">
+        <v>27223228</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
       <c r="A139" t="s">
         <v>175</v>
       </c>
       <c r="B139" s="1">
         <v>233717.142857142</v>
       </c>
-    </row>
-    <row r="140" spans="1:2">
+      <c r="C139" t="s">
+        <v>316</v>
+      </c>
+      <c r="D139" s="2">
+        <v>4630000</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
       <c r="A140" t="s">
         <v>109</v>
       </c>
       <c r="B140" s="1">
         <v>217500</v>
       </c>
-    </row>
-    <row r="141" spans="1:2">
+      <c r="C140" t="s">
+        <v>226</v>
+      </c>
+      <c r="D140" s="2">
+        <v>88340</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
       <c r="A141" t="s">
         <v>105</v>
       </c>
       <c r="B141" s="1">
         <v>214163.41666666599</v>
       </c>
-    </row>
-    <row r="142" spans="1:2">
+      <c r="C141" t="s">
+        <v>286</v>
+      </c>
+      <c r="D141" s="2">
+        <v>14790608</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
       <c r="A142" t="s">
         <v>131</v>
       </c>
       <c r="B142" s="1">
         <v>151433</v>
       </c>
-    </row>
-    <row r="143" spans="1:2">
+      <c r="C142" t="s">
+        <v>285</v>
+      </c>
+      <c r="D142" s="2">
+        <v>22912177</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
       <c r="A143" t="s">
         <v>176</v>
       </c>
       <c r="B143" s="1">
         <v>129532.666666666</v>
       </c>
-    </row>
-    <row r="144" spans="1:2">
+      <c r="C143" t="s">
+        <v>284</v>
+      </c>
+      <c r="D143" s="2">
+        <v>9823821</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
       <c r="A144" t="s">
         <v>99</v>
       </c>
       <c r="B144" s="1">
         <v>108201.25</v>
       </c>
-    </row>
-    <row r="145" spans="1:2">
+      <c r="C144" t="s">
+        <v>283</v>
+      </c>
+      <c r="D144" s="2">
+        <v>19294149</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
       <c r="A145" t="s">
         <v>91</v>
       </c>
       <c r="B145" s="1">
         <v>100000</v>
       </c>
-    </row>
-    <row r="146" spans="1:2">
+      <c r="C145" t="s">
+        <v>282</v>
+      </c>
+      <c r="D145" s="2">
+        <v>72813</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
       <c r="A146" t="s">
         <v>113</v>
       </c>
       <c r="B146" s="1">
         <v>90000</v>
       </c>
-    </row>
-    <row r="147" spans="1:2">
+      <c r="C146" t="s">
+        <v>281</v>
+      </c>
+      <c r="D146" s="2">
+        <v>27865738</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
       <c r="A147" t="s">
         <v>66</v>
       </c>
       <c r="B147" s="1">
         <v>54504</v>
       </c>
-    </row>
-    <row r="148" spans="1:2">
+      <c r="C147" t="s">
+        <v>280</v>
+      </c>
+      <c r="D147" s="2">
+        <v>776948</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
       <c r="A148" t="s">
         <v>162</v>
       </c>
       <c r="B148" s="1">
         <v>40306</v>
       </c>
-    </row>
-    <row r="149" spans="1:2">
+      <c r="C148" t="s">
+        <v>279</v>
+      </c>
+      <c r="D148" s="2">
+        <v>4590000</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
       <c r="A149" t="s">
         <v>65</v>
       </c>
       <c r="B149" s="1">
         <v>32800</v>
       </c>
-    </row>
-    <row r="150" spans="1:2">
+      <c r="C149" t="s">
+        <v>278</v>
+      </c>
+      <c r="D149" s="2">
+        <v>4324000</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
       <c r="A150" t="s">
         <v>145</v>
       </c>
       <c r="B150" s="1">
         <v>25000</v>
       </c>
-    </row>
-    <row r="151" spans="1:2">
+      <c r="C150" t="s">
+        <v>264</v>
+      </c>
+      <c r="D150" s="2">
+        <v>29671605</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
       <c r="A151" t="s">
         <v>88</v>
       </c>
       <c r="B151" s="1">
         <v>4500</v>
       </c>
+      <c r="C151" t="s">
+        <v>263</v>
+      </c>
+      <c r="D151" s="2">
+        <v>7989415</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D151"/>
+  <autoFilter ref="A1:D151">
+    <sortState ref="A2:D151">
+      <sortCondition descending="1" ref="B1:B151"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4940,1225 +5801,2135 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B151"/>
+  <dimension ref="A1:D151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>199</v>
       </c>
       <c r="B1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>146</v>
       </c>
       <c r="B2">
         <v>43095</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D2" s="2">
+        <v>310232863</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>116</v>
       </c>
       <c r="B3">
         <v>5393</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="s">
+        <v>262</v>
+      </c>
+      <c r="D3" s="2">
+        <v>62348447</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>126</v>
       </c>
       <c r="B4">
         <v>2420</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" t="s">
+        <v>252</v>
+      </c>
+      <c r="D4" s="2">
+        <v>33679000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>121</v>
       </c>
       <c r="B5">
         <v>2325</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1173108018</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>152</v>
       </c>
       <c r="B6">
         <v>1912</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1330044000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>186</v>
       </c>
       <c r="B7">
         <v>1563</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" t="s">
+        <v>260</v>
+      </c>
+      <c r="D7" s="2">
+        <v>64768389</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>54</v>
       </c>
       <c r="B8">
         <v>1244</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" t="s">
+        <v>239</v>
+      </c>
+      <c r="D8" s="2">
+        <v>81802257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>75</v>
       </c>
       <c r="B9">
         <v>1242</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" t="s">
+        <v>253</v>
+      </c>
+      <c r="D9" s="2">
+        <v>7353985</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>53</v>
       </c>
       <c r="B10">
         <v>941</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" t="s">
+        <v>245</v>
+      </c>
+      <c r="D10" s="2">
+        <v>46505963</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>138</v>
       </c>
       <c r="B11">
         <v>875</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11" t="s">
+        <v>258</v>
+      </c>
+      <c r="D11" s="2">
+        <v>21515754</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>184</v>
       </c>
       <c r="B12">
         <v>763</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12" t="s">
+        <v>257</v>
+      </c>
+      <c r="D12" s="2">
+        <v>9555893</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>132</v>
       </c>
       <c r="B13">
         <v>617</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" t="s">
+        <v>247</v>
+      </c>
+      <c r="D13" s="2">
+        <v>16654000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>122</v>
       </c>
       <c r="B14">
         <v>601</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14" t="s">
+        <v>232</v>
+      </c>
+      <c r="D14" s="2">
+        <v>4701069</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>144</v>
       </c>
       <c r="B15">
         <v>577</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15" t="s">
+        <v>219</v>
+      </c>
+      <c r="D15" s="2">
+        <v>140702000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>142</v>
       </c>
       <c r="B16">
         <v>565</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" t="s">
+        <v>261</v>
+      </c>
+      <c r="D16" s="2">
+        <v>201103330</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>170</v>
       </c>
       <c r="B17">
         <v>548</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" t="s">
+        <v>248</v>
+      </c>
+      <c r="D17" s="2">
+        <v>4622917</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>85</v>
       </c>
       <c r="B18">
         <v>543</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" t="s">
+        <v>292</v>
+      </c>
+      <c r="D18" s="2">
+        <v>60340328</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>60</v>
       </c>
       <c r="B19">
         <v>498</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" t="s">
+        <v>218</v>
+      </c>
+      <c r="D19" s="2">
+        <v>127288000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>134</v>
       </c>
       <c r="B20">
         <v>476</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" t="s">
+        <v>250</v>
+      </c>
+      <c r="D20" s="2">
+        <v>48422644</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>178</v>
       </c>
       <c r="B21">
         <v>449</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" t="s">
+        <v>287</v>
+      </c>
+      <c r="D21" s="2">
+        <v>7581000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>190</v>
       </c>
       <c r="B22">
         <v>385</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" t="s">
+        <v>288</v>
+      </c>
+      <c r="D22" s="2">
+        <v>5244000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>93</v>
       </c>
       <c r="B23">
         <v>350</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" t="s">
+        <v>270</v>
+      </c>
+      <c r="D23" s="2">
+        <v>5484000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>77</v>
       </c>
       <c r="B24">
         <v>348</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" t="s">
+        <v>311</v>
+      </c>
+      <c r="D24" s="2">
+        <v>16746491</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>80</v>
       </c>
       <c r="B25">
         <v>311</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" t="s">
+        <v>237</v>
+      </c>
+      <c r="D25" s="2">
+        <v>6898686</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>78</v>
       </c>
       <c r="B26">
         <v>302</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26" t="s">
+        <v>271</v>
+      </c>
+      <c r="D26" s="2">
+        <v>10403000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>110</v>
       </c>
       <c r="B27">
         <v>230</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" t="s">
+        <v>243</v>
+      </c>
+      <c r="D27" s="2">
+        <v>38500000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>95</v>
       </c>
       <c r="B28">
         <v>226</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" t="s">
+        <v>273</v>
+      </c>
+      <c r="D28" s="2">
+        <v>112468855</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>76</v>
       </c>
       <c r="B29">
         <v>219</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" t="s">
+        <v>337</v>
+      </c>
+      <c r="D29" s="2">
+        <v>41343201</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>137</v>
       </c>
       <c r="B30">
         <v>199</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30" t="s">
+        <v>293</v>
+      </c>
+      <c r="D30" s="2">
+        <v>77804122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>187</v>
       </c>
       <c r="B31">
         <v>197</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31" t="s">
+        <v>321</v>
+      </c>
+      <c r="D31" s="2">
+        <v>308910</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>147</v>
       </c>
       <c r="B32">
         <v>190</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" t="s">
+        <v>256</v>
+      </c>
+      <c r="D32" s="2">
+        <v>5009150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>155</v>
       </c>
       <c r="B33">
         <v>162</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" t="s">
+        <v>269</v>
+      </c>
+      <c r="D33" s="2">
+        <v>8205000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>171</v>
       </c>
       <c r="B34">
         <v>151</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34" t="s">
+        <v>223</v>
+      </c>
+      <c r="D34" s="2">
+        <v>4975593</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>150</v>
       </c>
       <c r="B35">
         <v>148</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" t="s">
+        <v>265</v>
+      </c>
+      <c r="D35" s="2">
+        <v>28274729</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>98</v>
       </c>
       <c r="B36">
         <v>147</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36" t="s">
+        <v>215</v>
+      </c>
+      <c r="D36" s="2">
+        <v>49000000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>167</v>
       </c>
       <c r="B37">
         <v>141</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37" t="s">
+        <v>251</v>
+      </c>
+      <c r="D37" s="2">
+        <v>4252277</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>153</v>
       </c>
       <c r="B38">
         <v>134</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38" t="s">
+        <v>350</v>
+      </c>
+      <c r="D38" s="2">
+        <v>10676000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>168</v>
       </c>
       <c r="B39">
         <v>132</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39" t="s">
+        <v>304</v>
+      </c>
+      <c r="D39" s="2">
+        <v>7148785</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>64</v>
       </c>
       <c r="B40">
         <v>123</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40" t="s">
+        <v>353</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1291170</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>127</v>
       </c>
       <c r="B41">
         <v>119</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="C41" t="s">
+        <v>294</v>
+      </c>
+      <c r="D41" s="2">
+        <v>45415596</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>104</v>
       </c>
       <c r="B42">
         <v>116</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="C42" t="s">
+        <v>221</v>
+      </c>
+      <c r="D42" s="2">
+        <v>242968342</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>61</v>
       </c>
       <c r="B43">
         <v>112</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43" t="s">
+        <v>233</v>
+      </c>
+      <c r="D43" s="2">
+        <v>122580</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>101</v>
       </c>
       <c r="B44">
         <v>98</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="C44" t="s">
+        <v>249</v>
+      </c>
+      <c r="D44" s="2">
+        <v>22894384</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>123</v>
       </c>
       <c r="B45">
         <v>95</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="C45" t="s">
+        <v>276</v>
+      </c>
+      <c r="D45" s="2">
+        <v>10476000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>69</v>
       </c>
       <c r="B46">
         <v>86</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="C46" t="s">
+        <v>267</v>
+      </c>
+      <c r="D46" s="2">
+        <v>47790000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>120</v>
       </c>
       <c r="B47">
         <v>84</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="C47" t="s">
+        <v>240</v>
+      </c>
+      <c r="D47" s="2">
+        <v>67089500</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>59</v>
       </c>
       <c r="B48">
         <v>81</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="C48" t="s">
+        <v>216</v>
+      </c>
+      <c r="D48" s="2">
+        <v>99900177</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>94</v>
       </c>
       <c r="B49">
         <v>77</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="C49" t="s">
+        <v>217</v>
+      </c>
+      <c r="D49" s="2">
+        <v>40046566</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>189</v>
       </c>
       <c r="B50">
         <v>76</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="C50" t="s">
+        <v>317</v>
+      </c>
+      <c r="D50" s="2">
+        <v>9932000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>92</v>
       </c>
       <c r="B51">
         <v>72</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="C51" t="s">
+        <v>254</v>
+      </c>
+      <c r="D51" s="2">
+        <v>80471869</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>149</v>
       </c>
       <c r="B52">
         <v>71</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="C52" t="s">
+        <v>272</v>
+      </c>
+      <c r="D52" s="2">
+        <v>2217969</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>107</v>
       </c>
       <c r="B53">
         <v>70</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="C53" t="s">
+        <v>246</v>
+      </c>
+      <c r="D53" s="2">
+        <v>89571130</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>163</v>
       </c>
       <c r="B54">
         <v>66</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="C54" t="s">
+        <v>327</v>
+      </c>
+      <c r="D54" s="2">
+        <v>11000000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>117</v>
       </c>
       <c r="B55">
         <v>65</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="C55" t="s">
+        <v>319</v>
+      </c>
+      <c r="D55" s="2">
+        <v>21959278</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>166</v>
       </c>
       <c r="B56">
         <v>59</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="C56" t="s">
+        <v>340</v>
+      </c>
+      <c r="D56" s="2">
+        <v>2944459</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>79</v>
       </c>
       <c r="B57">
         <v>58</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="C57" t="s">
+        <v>352</v>
+      </c>
+      <c r="D57" s="2">
+        <v>29907003</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>119</v>
       </c>
       <c r="B58">
         <v>43</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="C58" t="s">
+        <v>224</v>
+      </c>
+      <c r="D58" s="2">
+        <v>497538</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="B59">
         <v>41</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="C59" t="s">
+        <v>275</v>
+      </c>
+      <c r="D59" s="2">
+        <v>184404791</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="B60">
         <v>41</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="C60" t="s">
+        <v>296</v>
+      </c>
+      <c r="D60" s="2">
+        <v>2007000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
         <v>108</v>
       </c>
       <c r="B61">
         <v>38</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
+      <c r="C61" t="s">
+        <v>320</v>
+      </c>
+      <c r="D61" s="2">
+        <v>5455000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
         <v>81</v>
       </c>
       <c r="B62">
         <v>36</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
+      <c r="C62" t="s">
+        <v>326</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1102677</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
         <v>114</v>
       </c>
       <c r="B63">
         <v>36</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
+      <c r="C63" t="s">
+        <v>322</v>
+      </c>
+      <c r="D63" s="2">
+        <v>4125247</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
         <v>140</v>
       </c>
       <c r="B64">
         <v>34</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
+      <c r="C64" t="s">
+        <v>339</v>
+      </c>
+      <c r="D64" s="2">
+        <v>6407085</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>83</v>
       </c>
       <c r="B65">
         <v>24</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
+      <c r="C65" t="s">
+        <v>338</v>
+      </c>
+      <c r="D65" s="2">
+        <v>31627428</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>89</v>
       </c>
       <c r="B66">
         <v>23</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
+      <c r="C66" t="s">
+        <v>307</v>
+      </c>
+      <c r="D66" s="2">
+        <v>7344847</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>96</v>
       </c>
       <c r="B67">
         <v>21</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
+      <c r="C67" t="s">
+        <v>291</v>
+      </c>
+      <c r="D67" s="2">
+        <v>156118464</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>181</v>
       </c>
       <c r="B68">
         <v>21</v>
       </c>
-    </row>
-    <row r="69" spans="1:2">
+      <c r="C68" t="s">
+        <v>343</v>
+      </c>
+      <c r="D68" s="2">
+        <v>24339838</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
         <v>56</v>
       </c>
       <c r="B69">
         <v>20</v>
       </c>
-    </row>
-    <row r="70" spans="1:2">
+      <c r="C69" t="s">
+        <v>315</v>
+      </c>
+      <c r="D69" s="2">
+        <v>27223228</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>118</v>
       </c>
       <c r="B70">
         <v>19</v>
       </c>
-    </row>
-    <row r="71" spans="1:2">
+      <c r="C70" t="s">
+        <v>329</v>
+      </c>
+      <c r="D70" s="2">
+        <v>33398682</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
         <v>129</v>
       </c>
       <c r="B71">
         <v>17</v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
+      <c r="C71" t="s">
+        <v>242</v>
+      </c>
+      <c r="D71" s="2">
+        <v>44270</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
         <v>143</v>
       </c>
       <c r="B72">
         <v>16</v>
       </c>
-    </row>
-    <row r="73" spans="1:2">
+      <c r="C72" t="s">
+        <v>301</v>
+      </c>
+      <c r="D72" s="2">
+        <v>4491000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>192</v>
       </c>
       <c r="B73">
         <v>16</v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
+      <c r="C73" t="s">
+        <v>295</v>
+      </c>
+      <c r="D73" s="2">
+        <v>25731776</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>50</v>
+        <v>148</v>
       </c>
       <c r="B74">
         <v>15</v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
+      <c r="C74" t="s">
+        <v>346</v>
+      </c>
+      <c r="D74" s="2">
+        <v>403000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="B75">
         <v>15</v>
       </c>
-    </row>
-    <row r="76" spans="1:2">
+      <c r="C75" t="s">
+        <v>325</v>
+      </c>
+      <c r="D75" s="2">
+        <v>41892895</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>148</v>
+        <v>90</v>
       </c>
       <c r="B76">
         <v>15</v>
       </c>
-    </row>
-    <row r="77" spans="1:2">
+      <c r="C76" t="s">
+        <v>318</v>
+      </c>
+      <c r="D76" s="2">
+        <v>3477000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>74</v>
+        <v>165</v>
       </c>
       <c r="B77">
         <v>14</v>
       </c>
-    </row>
-    <row r="78" spans="1:2">
+      <c r="C77" t="s">
+        <v>306</v>
+      </c>
+      <c r="D77" s="2">
+        <v>4516220</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
         <v>115</v>
       </c>
       <c r="B78">
         <v>14</v>
       </c>
-    </row>
-    <row r="79" spans="1:2">
+      <c r="C78" t="s">
+        <v>209</v>
+      </c>
+      <c r="D78" s="2">
+        <v>1294104</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>165</v>
+        <v>74</v>
       </c>
       <c r="B79">
         <v>14</v>
       </c>
-    </row>
-    <row r="80" spans="1:2">
+      <c r="C79" t="s">
+        <v>351</v>
+      </c>
+      <c r="D79" s="2">
+        <v>3410676</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
         <v>73</v>
       </c>
       <c r="B80">
         <v>13</v>
       </c>
-    </row>
-    <row r="81" spans="1:2">
+      <c r="C80" t="s">
+        <v>303</v>
+      </c>
+      <c r="D80" s="2">
+        <v>8303512</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81" t="s">
         <v>196</v>
       </c>
       <c r="B81">
         <v>13</v>
       </c>
-    </row>
-    <row r="82" spans="1:2">
+      <c r="C81" t="s">
+        <v>208</v>
+      </c>
+      <c r="D81" s="2">
+        <v>65365</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82" t="s">
         <v>70</v>
       </c>
       <c r="B82">
         <v>12</v>
       </c>
-    </row>
-    <row r="83" spans="1:2">
+      <c r="C82" t="s">
+        <v>238</v>
+      </c>
+      <c r="D82" s="2">
+        <v>2968000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" t="s">
         <v>105</v>
       </c>
       <c r="B83">
         <v>12</v>
       </c>
-    </row>
-    <row r="84" spans="1:2">
+      <c r="C83" t="s">
+        <v>286</v>
+      </c>
+      <c r="D83" s="2">
+        <v>14790608</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84" t="s">
         <v>197</v>
       </c>
       <c r="B84">
         <v>12</v>
       </c>
-    </row>
-    <row r="85" spans="1:2">
+      <c r="C84" t="s">
+        <v>323</v>
+      </c>
+      <c r="D84" s="2">
+        <v>53414374</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85" t="s">
         <v>194</v>
       </c>
       <c r="B85">
         <v>11</v>
       </c>
-    </row>
-    <row r="86" spans="1:2">
+      <c r="C85" t="s">
+        <v>309</v>
+      </c>
+      <c r="D85" s="2">
+        <v>9685000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86" t="s">
         <v>71</v>
       </c>
       <c r="B86">
         <v>9</v>
       </c>
-    </row>
-    <row r="87" spans="1:2">
+      <c r="C86" t="s">
+        <v>342</v>
+      </c>
+      <c r="D86" s="2">
+        <v>21513990</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87" t="s">
         <v>188</v>
       </c>
       <c r="B87">
         <v>8</v>
       </c>
-    </row>
-    <row r="88" spans="1:2">
+      <c r="C87" t="s">
+        <v>220</v>
+      </c>
+      <c r="D87" s="2">
+        <v>76923000</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>62</v>
+        <v>175</v>
       </c>
       <c r="B88">
         <v>7</v>
       </c>
-    </row>
-    <row r="89" spans="1:2">
+      <c r="C88" t="s">
+        <v>316</v>
+      </c>
+      <c r="D88" s="2">
+        <v>4630000</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="B89">
         <v>7</v>
       </c>
-    </row>
-    <row r="90" spans="1:2">
+      <c r="C89" t="s">
+        <v>336</v>
+      </c>
+      <c r="D89" s="2">
+        <v>13550440</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>157</v>
+        <v>195</v>
       </c>
       <c r="B90">
         <v>7</v>
       </c>
-    </row>
-    <row r="91" spans="1:2">
+      <c r="C90" t="s">
+        <v>302</v>
+      </c>
+      <c r="D90" s="2">
+        <v>14453680</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>174</v>
+        <v>62</v>
       </c>
       <c r="B91">
         <v>7</v>
       </c>
-    </row>
-    <row r="92" spans="1:2">
+      <c r="C91" t="s">
+        <v>354</v>
+      </c>
+      <c r="D91" s="2">
+        <v>28951852</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>175</v>
+        <v>125</v>
       </c>
       <c r="B92">
         <v>7</v>
       </c>
-    </row>
-    <row r="93" spans="1:2">
+      <c r="C92" t="s">
+        <v>348</v>
+      </c>
+      <c r="D92" s="2">
+        <v>3916632</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
       <c r="A93" t="s">
         <v>185</v>
       </c>
       <c r="B93">
         <v>7</v>
       </c>
-    </row>
-    <row r="94" spans="1:2">
+      <c r="C93" t="s">
+        <v>335</v>
+      </c>
+      <c r="D93" s="2">
+        <v>1228691</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="B94">
         <v>7</v>
       </c>
-    </row>
-    <row r="95" spans="1:2">
+      <c r="C94" t="s">
+        <v>330</v>
+      </c>
+      <c r="D94" s="2">
+        <v>10589025</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95" t="s">
         <v>103</v>
       </c>
       <c r="B95">
         <v>6</v>
       </c>
-    </row>
-    <row r="96" spans="1:2">
+      <c r="C95" t="s">
+        <v>274</v>
+      </c>
+      <c r="D95" s="2">
+        <v>21058798</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="B96">
         <v>6</v>
       </c>
-    </row>
-    <row r="97" spans="1:2">
+      <c r="C96" t="s">
+        <v>231</v>
+      </c>
+      <c r="D96" s="2">
+        <v>90812</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="B97">
         <v>6</v>
       </c>
-    </row>
-    <row r="98" spans="1:2">
+      <c r="C97" t="s">
+        <v>298</v>
+      </c>
+      <c r="D97" s="2">
+        <v>2062294</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="B98">
         <v>6</v>
       </c>
-    </row>
-    <row r="99" spans="1:2">
+      <c r="C98" t="s">
+        <v>300</v>
+      </c>
+      <c r="D98" s="2">
+        <v>6052064</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="B99">
         <v>6</v>
       </c>
-    </row>
-    <row r="100" spans="1:2">
+      <c r="C99" t="s">
+        <v>244</v>
+      </c>
+      <c r="D99" s="2">
+        <v>11651858</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="B100">
         <v>5</v>
       </c>
-    </row>
-    <row r="101" spans="1:2">
+      <c r="C100" t="s">
+        <v>212</v>
+      </c>
+      <c r="D100" s="2">
+        <v>88013491</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="B101">
         <v>5</v>
       </c>
-    </row>
-    <row r="102" spans="1:2">
+      <c r="C101" t="s">
+        <v>332</v>
+      </c>
+      <c r="D101" s="2">
+        <v>2789132</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
       <c r="A102" t="s">
         <v>86</v>
       </c>
       <c r="B102">
         <v>5</v>
       </c>
-    </row>
-    <row r="103" spans="1:2">
+      <c r="C102" t="s">
+        <v>213</v>
+      </c>
+      <c r="D102" s="2">
+        <v>840926</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B103">
         <v>5</v>
       </c>
-    </row>
-    <row r="104" spans="1:2">
+      <c r="C103" t="s">
+        <v>297</v>
+      </c>
+      <c r="D103" s="2">
+        <v>11055976</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
       <c r="A104" t="s">
         <v>193</v>
       </c>
       <c r="B104">
         <v>5</v>
       </c>
-    </row>
-    <row r="105" spans="1:2">
+      <c r="C104" t="s">
+        <v>313</v>
+      </c>
+      <c r="D104" s="2">
+        <v>13460305</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>51</v>
+        <v>111</v>
       </c>
       <c r="B105">
         <v>4</v>
       </c>
-    </row>
-    <row r="106" spans="1:2">
+      <c r="C105" t="s">
+        <v>341</v>
+      </c>
+      <c r="D105" s="2">
+        <v>2986952</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
       <c r="A106" t="s">
         <v>99</v>
       </c>
       <c r="B106">
         <v>4</v>
       </c>
-    </row>
-    <row r="107" spans="1:2">
+      <c r="C106" t="s">
+        <v>283</v>
+      </c>
+      <c r="D106" s="2">
+        <v>19294149</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
       <c r="A107" t="s">
-        <v>100</v>
+        <v>191</v>
       </c>
       <c r="B107">
         <v>4</v>
       </c>
-    </row>
-    <row r="108" spans="1:2">
+      <c r="C107" t="s">
+        <v>255</v>
+      </c>
+      <c r="D107" s="2">
+        <v>27884</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>111</v>
+        <v>51</v>
       </c>
       <c r="B108">
         <v>4</v>
       </c>
-    </row>
-    <row r="109" spans="1:2">
+      <c r="C108" t="s">
+        <v>214</v>
+      </c>
+      <c r="D108" s="2">
+        <v>2967717</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
       <c r="A109" t="s">
         <v>180</v>
       </c>
       <c r="B109">
         <v>4</v>
       </c>
-    </row>
-    <row r="110" spans="1:2">
+      <c r="C109" t="s">
+        <v>345</v>
+      </c>
+      <c r="D109" s="2">
+        <v>3800000</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>191</v>
+        <v>100</v>
       </c>
       <c r="B110">
         <v>4</v>
       </c>
-    </row>
-    <row r="111" spans="1:2">
+      <c r="C110" t="s">
+        <v>328</v>
+      </c>
+      <c r="D110" s="2">
+        <v>12323252</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B111">
         <v>3</v>
       </c>
-    </row>
-    <row r="112" spans="1:2">
+      <c r="C111" t="s">
+        <v>334</v>
+      </c>
+      <c r="D111" s="2">
+        <v>301790</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
       <c r="A112" t="s">
-        <v>72</v>
+        <v>139</v>
       </c>
       <c r="B112">
         <v>3</v>
       </c>
-    </row>
-    <row r="113" spans="1:2">
+      <c r="C112" t="s">
+        <v>268</v>
+      </c>
+      <c r="D112" s="2">
+        <v>738004</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>97</v>
+        <v>156</v>
       </c>
       <c r="B113">
         <v>3</v>
       </c>
-    </row>
-    <row r="114" spans="1:2">
+      <c r="C113" t="s">
+        <v>266</v>
+      </c>
+      <c r="D113" s="2">
+        <v>70916439</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>130</v>
+        <v>176</v>
       </c>
       <c r="B114">
         <v>3</v>
       </c>
-    </row>
-    <row r="115" spans="1:2">
+      <c r="C114" t="s">
+        <v>284</v>
+      </c>
+      <c r="D114" s="2">
+        <v>9823821</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="B115">
         <v>3</v>
       </c>
-    </row>
-    <row r="116" spans="1:2">
+      <c r="C115" t="s">
+        <v>205</v>
+      </c>
+      <c r="D115" s="2">
+        <v>2847232</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B116">
         <v>3</v>
       </c>
-    </row>
-    <row r="117" spans="1:2">
+      <c r="C116" t="s">
+        <v>308</v>
+      </c>
+      <c r="D116" s="2">
+        <v>15340000</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="B117">
         <v>3</v>
       </c>
-    </row>
-    <row r="118" spans="1:2">
+      <c r="C117" t="s">
+        <v>290</v>
+      </c>
+      <c r="D117" s="2">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>172</v>
+        <v>130</v>
       </c>
       <c r="B118">
         <v>3</v>
       </c>
-    </row>
-    <row r="119" spans="1:2">
+      <c r="C118" t="s">
+        <v>299</v>
+      </c>
+      <c r="D118" s="2">
+        <v>32965</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>173</v>
+        <v>65</v>
       </c>
       <c r="B119">
         <v>3</v>
       </c>
-    </row>
-    <row r="120" spans="1:2">
+      <c r="C119" t="s">
+        <v>278</v>
+      </c>
+      <c r="D119" s="2">
+        <v>4324000</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>176</v>
+        <v>97</v>
       </c>
       <c r="B120">
         <v>3</v>
       </c>
-    </row>
-    <row r="121" spans="1:2">
+      <c r="C120" t="s">
+        <v>206</v>
+      </c>
+      <c r="D120" s="2">
+        <v>6587239</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
       <c r="A121" t="s">
-        <v>55</v>
+        <v>162</v>
       </c>
       <c r="B121">
         <v>2</v>
       </c>
-    </row>
-    <row r="122" spans="1:2">
+      <c r="C121" t="s">
+        <v>279</v>
+      </c>
+      <c r="D121" s="2">
+        <v>4590000</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B122">
         <v>2</v>
       </c>
-    </row>
-    <row r="123" spans="1:2">
+      <c r="C122" t="s">
+        <v>310</v>
+      </c>
+      <c r="D122" s="2">
+        <v>2029307</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>68</v>
+        <v>151</v>
       </c>
       <c r="B123">
         <v>2</v>
       </c>
-    </row>
-    <row r="124" spans="1:2">
+      <c r="C123" t="s">
+        <v>229</v>
+      </c>
+      <c r="D123" s="2">
+        <v>34586184</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
       <c r="A124" t="s">
-        <v>109</v>
+        <v>179</v>
       </c>
       <c r="B124">
         <v>2</v>
       </c>
-    </row>
-    <row r="125" spans="1:2">
+      <c r="C124" t="s">
+        <v>331</v>
+      </c>
+      <c r="D124" s="2">
+        <v>65228</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
       <c r="A125" t="s">
         <v>124</v>
       </c>
       <c r="B125">
         <v>2</v>
       </c>
-    </row>
-    <row r="126" spans="1:2">
+      <c r="C125" t="s">
+        <v>241</v>
+      </c>
+      <c r="D125" s="2">
+        <v>13796354</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>131</v>
+        <v>63</v>
       </c>
       <c r="B126">
         <v>2</v>
       </c>
-    </row>
-    <row r="127" spans="1:2">
+      <c r="C126" t="s">
+        <v>312</v>
+      </c>
+      <c r="D126" s="2">
+        <v>22061451</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
       <c r="A127" t="s">
-        <v>151</v>
+        <v>55</v>
       </c>
       <c r="B127">
         <v>2</v>
       </c>
-    </row>
-    <row r="128" spans="1:2">
+      <c r="C127" t="s">
+        <v>305</v>
+      </c>
+      <c r="D127" s="2">
+        <v>5995928</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
       <c r="A128" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
       <c r="B128">
         <v>2</v>
       </c>
-    </row>
-    <row r="129" spans="1:2">
+      <c r="C128" t="s">
+        <v>285</v>
+      </c>
+      <c r="D128" s="2">
+        <v>22912177</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
       <c r="A129" t="s">
         <v>169</v>
       </c>
       <c r="B129">
         <v>2</v>
       </c>
-    </row>
-    <row r="130" spans="1:2">
+      <c r="C129" t="s">
+        <v>333</v>
+      </c>
+      <c r="D129" s="2">
+        <v>6375830</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
       <c r="A130" t="s">
-        <v>179</v>
+        <v>109</v>
       </c>
       <c r="B130">
         <v>2</v>
       </c>
-    </row>
-    <row r="131" spans="1:2">
+      <c r="C130" t="s">
+        <v>226</v>
+      </c>
+      <c r="D130" s="2">
+        <v>88340</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
       <c r="A131" t="s">
-        <v>49</v>
+        <v>102</v>
       </c>
       <c r="B131">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:2">
+      <c r="C131" t="s">
+        <v>314</v>
+      </c>
+      <c r="D131" s="2">
+        <v>314522</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
       <c r="A132" t="s">
-        <v>52</v>
+        <v>135</v>
       </c>
       <c r="B132">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:2">
+      <c r="C132" t="s">
+        <v>277</v>
+      </c>
+      <c r="D132" s="2">
+        <v>286653</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
       <c r="A133" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="B133">
         <v>1</v>
       </c>
-    </row>
-    <row r="134" spans="1:2">
+      <c r="C133" t="s">
+        <v>211</v>
+      </c>
+      <c r="D133" s="2">
+        <v>3039126</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
       <c r="A134" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B134">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:2">
+      <c r="C134" t="s">
+        <v>225</v>
+      </c>
+      <c r="D134" s="2">
+        <v>740528</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
       <c r="A135" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="B135">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:2">
+      <c r="C135" t="s">
+        <v>282</v>
+      </c>
+      <c r="D135" s="2">
+        <v>72813</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
       <c r="A136" t="s">
-        <v>82</v>
+        <v>183</v>
       </c>
       <c r="B136">
         <v>1</v>
       </c>
-    </row>
-    <row r="137" spans="1:2">
+      <c r="C136" t="s">
+        <v>204</v>
+      </c>
+      <c r="D136" s="2">
+        <v>107818</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
       <c r="A137" t="s">
         <v>88</v>
       </c>
       <c r="B137">
         <v>1</v>
       </c>
-    </row>
-    <row r="138" spans="1:2">
+      <c r="C137" t="s">
+        <v>263</v>
+      </c>
+      <c r="D137" s="2">
+        <v>7989415</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
       <c r="A138" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B138">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="1:2">
+      <c r="C138" t="s">
+        <v>344</v>
+      </c>
+      <c r="D138" s="2">
+        <v>96489245</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
       <c r="A139" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="B139">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="1:2">
+      <c r="C139" t="s">
+        <v>289</v>
+      </c>
+      <c r="D139" s="2">
+        <v>75049</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
       <c r="A140" t="s">
-        <v>106</v>
+        <v>145</v>
       </c>
       <c r="B140">
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:2">
+      <c r="C140" t="s">
+        <v>264</v>
+      </c>
+      <c r="D140" s="2">
+        <v>29671605</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
       <c r="A141" t="s">
-        <v>113</v>
+        <v>164</v>
       </c>
       <c r="B141">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:2">
+      <c r="C141" t="s">
+        <v>347</v>
+      </c>
+      <c r="D141" s="2">
+        <v>6368162</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
       <c r="A142" t="s">
-        <v>128</v>
+        <v>159</v>
       </c>
       <c r="B142">
         <v>1</v>
       </c>
-    </row>
-    <row r="143" spans="1:2">
+      <c r="C142" t="s">
+        <v>235</v>
+      </c>
+      <c r="D142" s="2">
+        <v>3685076</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
       <c r="A143" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="B143">
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="1:2">
+      <c r="C143" t="s">
+        <v>227</v>
+      </c>
+      <c r="D143" s="2">
+        <v>35295</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
       <c r="A144" t="s">
-        <v>145</v>
+        <v>58</v>
       </c>
       <c r="B144">
         <v>1</v>
       </c>
-    </row>
-    <row r="145" spans="1:2">
+      <c r="C144" t="s">
+        <v>228</v>
+      </c>
+      <c r="D144" s="2">
+        <v>21281844</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
       <c r="A145" t="s">
-        <v>158</v>
+        <v>67</v>
       </c>
       <c r="B145">
         <v>1</v>
       </c>
-    </row>
-    <row r="146" spans="1:2">
+      <c r="C145" t="s">
+        <v>259</v>
+      </c>
+      <c r="D145" s="2">
+        <v>666730</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
       <c r="A146" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B146">
         <v>1</v>
       </c>
-    </row>
-    <row r="147" spans="1:2">
+      <c r="C146" t="s">
+        <v>324</v>
+      </c>
+      <c r="D146" s="2">
+        <v>386486</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
       <c r="A147" t="s">
-        <v>160</v>
+        <v>66</v>
       </c>
       <c r="B147">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="1:2">
+      <c r="C147" t="s">
+        <v>280</v>
+      </c>
+      <c r="D147" s="2">
+        <v>776948</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
       <c r="A148" t="s">
         <v>161</v>
       </c>
       <c r="B148">
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="1:2">
+      <c r="C148" t="s">
+        <v>236</v>
+      </c>
+      <c r="D148" s="2">
+        <v>5245695</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
       <c r="A149" t="s">
-        <v>164</v>
+        <v>128</v>
       </c>
       <c r="B149">
         <v>1</v>
       </c>
-    </row>
-    <row r="150" spans="1:2">
+      <c r="C149" t="s">
+        <v>349</v>
+      </c>
+      <c r="D149" s="2">
+        <v>10112453</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
       <c r="A150" t="s">
-        <v>177</v>
+        <v>106</v>
       </c>
       <c r="B150">
         <v>1</v>
       </c>
-    </row>
-    <row r="151" spans="1:2">
+      <c r="C150" t="s">
+        <v>207</v>
+      </c>
+      <c r="D150" s="2">
+        <v>175808</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
       <c r="A151" t="s">
-        <v>183</v>
+        <v>113</v>
       </c>
       <c r="B151">
         <v>1</v>
       </c>
+      <c r="C151" t="s">
+        <v>281</v>
+      </c>
+      <c r="D151" s="2">
+        <v>27865738</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B151">
-    <sortState ref="A2:B151">
+  <autoFilter ref="A1:D151">
+    <sortState ref="A2:D151">
       <sortCondition descending="1" ref="B1:B151"/>
     </sortState>
   </autoFilter>
@@ -7916,7 +9687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>